<commit_message>
Updated CLV calculation example spreadsheet
</commit_message>
<xml_diff>
--- a/CLV_calculation_example.xlsx
+++ b/CLV_calculation_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Revenue</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Number of customers</t>
   </si>
   <si>
-    <t>Retention rate (1-churn rate)</t>
-  </si>
-  <si>
-    <t>Discount rate</t>
-  </si>
-  <si>
     <t>Average span of life-time</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>Variable costs</t>
   </si>
   <si>
-    <t>Retention costs</t>
-  </si>
-  <si>
     <t>Discounted profit/customer</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>Average number of customers in period.</t>
   </si>
   <si>
-    <t>Retention rate</t>
-  </si>
-  <si>
     <t>A proportion of customers expected to remain with a company at a given month.</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t>The duration can be estimated in multiple ways including the use of historical data, expected retenion rate and other methods.</t>
   </si>
   <si>
-    <t>Monthly discount rate</t>
-  </si>
-  <si>
     <t>Months to discount</t>
   </si>
   <si>
@@ -175,6 +160,36 @@
   </si>
   <si>
     <t>The second term of the right side of the equation without retention costs (M).</t>
+  </si>
+  <si>
+    <t>Retention costs (M)</t>
+  </si>
+  <si>
+    <t>Monthly discount rate (d)</t>
+  </si>
+  <si>
+    <t>Average span of life-time (n)</t>
+  </si>
+  <si>
+    <t>Total GC</t>
+  </si>
+  <si>
+    <t>CLV in 3 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Gross contribution (GC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retention rate (r) </t>
+  </si>
+  <si>
+    <t>Discount rate (d)</t>
+  </si>
+  <si>
+    <t>A type of profit generated by customer, calculated as revenue less variable costs.</t>
   </si>
 </sst>
 </file>
@@ -308,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -347,6 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1109,13 +1125,13 @@
   <sheetData>
     <row r="2" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="32" x14ac:dyDescent="0.2">
@@ -1123,10 +1139,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -1136,10 +1152,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="25"/>
     </row>
@@ -1149,11 +1165,11 @@
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>18</v>
+      <c r="B7" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D7" s="25"/>
     </row>
@@ -1164,10 +1180,10 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" s="25"/>
     </row>
@@ -1176,31 +1192,29 @@
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>45</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
     </row>
-    <row r="13" spans="2:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -1208,15 +1222,15 @@
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -1224,14 +1238,16 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
@@ -1240,14 +1256,12 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>47</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
@@ -1256,13 +1270,13 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
@@ -1272,12 +1286,14 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
@@ -1286,10 +1302,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D25" s="25"/>
     </row>
@@ -1300,10 +1316,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D27" s="25"/>
     </row>
@@ -1314,10 +1330,10 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D29" s="25"/>
     </row>
@@ -1328,10 +1344,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" s="25"/>
     </row>
@@ -1342,30 +1358,44 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="25"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="25"/>
-    </row>
-    <row r="35" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="27"/>
+      <c r="C37" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1374,18 +1404,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AK44"/>
+  <dimension ref="A2:AL49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="3" max="36" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1578,7 +1608,7 @@
     </row>
     <row r="5" spans="1:37" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="14"/>
     </row>
@@ -1735,7 +1765,7 @@
     </row>
     <row r="8" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6">
         <v>4775.5768494136473</v>
@@ -1886,7 +1916,7 @@
     </row>
     <row r="10" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B10" s="6">
         <v>8998.0768494136464</v>
@@ -2187,8 +2217,9 @@
       <c r="AK13" s="7"/>
     </row>
     <row r="14" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>2</v>
+      <c r="A14" s="5" t="str">
+        <f>"Retention rate (r) (1-churn rate)"</f>
+        <v>Retention rate (r) (1-churn rate)</v>
       </c>
       <c r="B14" s="8">
         <f>90%*(98%/90%)^(1/36)</f>
@@ -2409,12 +2440,12 @@
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8"/>
     </row>
-    <row r="17" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2451,9 +2482,9 @@
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B19" s="23">
         <f>(1+13%)^(1/12)-1</f>
@@ -2494,7 +2525,7 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
     </row>
-    <row r="20" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2531,9 +2562,9 @@
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8"/>
     </row>
-    <row r="21" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B21" s="6">
         <v>4</v>
@@ -2573,7 +2604,7 @@
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
     </row>
-    <row r="22" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2610,7 +2641,7 @@
       <c r="AI22" s="7"/>
       <c r="AJ22" s="7"/>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2647,12 +2678,12 @@
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
     </row>
-    <row r="24" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2689,9 +2720,9 @@
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
     </row>
-    <row r="26" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26" s="6">
         <f>COUNT($B$2:B2)</f>
@@ -2838,7 +2869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -2875,9 +2906,9 @@
       <c r="AI27" s="6"/>
       <c r="AJ27" s="6"/>
     </row>
-    <row r="28" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28" s="7">
         <f>B14/((1+$B$19)^(B26))</f>
@@ -3024,7 +3055,7 @@
         <v>7.5455514556023576E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -3062,9 +3093,9 @@
       <c r="AJ29" s="7"/>
       <c r="AK29" s="7"/>
     </row>
-    <row r="30" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="7">
         <f>B14/((1+$B$19)^(B26-(0.5/12)))</f>
@@ -3211,7 +3242,7 @@
         <v>7.5487542165037211E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -3249,156 +3280,157 @@
       <c r="AJ31" s="6"/>
       <c r="AK31" s="6"/>
     </row>
-    <row r="32" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B32" s="6">
-        <f>(B6-B8)/B12</f>
-        <v>13.989181645836057</v>
+        <f>B6-B8</f>
+        <v>9219.6080919510969</v>
       </c>
       <c r="C32" s="6">
-        <f>(C6-C8)/C12</f>
-        <v>14.841496961572126</v>
+        <f t="shared" ref="C32:AK32" si="1">C6-C8</f>
+        <v>10943.856366060891</v>
       </c>
       <c r="D32" s="6">
-        <f>(D6-D8)/D12</f>
-        <v>15.549784949153652</v>
+        <f t="shared" si="1"/>
+        <v>12681.773126547196</v>
       </c>
       <c r="E32" s="6">
-        <f>(E6-E8)/E12</f>
-        <v>16.151804880276416</v>
+        <f t="shared" si="1"/>
+        <v>14431.654619281348</v>
       </c>
       <c r="F32" s="6">
-        <f>(F6-F8)/F12</f>
-        <v>16.673179435248599</v>
+        <f t="shared" si="1"/>
+        <v>16191.577258721845</v>
       </c>
       <c r="G32" s="6">
-        <f>(G6-G8)/G12</f>
-        <v>15.448216578622993</v>
+        <f t="shared" si="1"/>
+        <v>16194.353030546554</v>
       </c>
       <c r="H32" s="6">
-        <f>(H6-H8)/H12</f>
-        <v>15.971976550004259</v>
+        <f t="shared" si="1"/>
+        <v>17967.505849915371</v>
       </c>
       <c r="I32" s="6">
-        <f>(I6-I8)/I12</f>
-        <v>16.440239087149006</v>
+        <f t="shared" si="1"/>
+        <v>19743.246292164047</v>
       </c>
       <c r="J32" s="6">
-        <f>(J6-J8)/J12</f>
-        <v>16.863034909542908</v>
+        <f t="shared" si="1"/>
+        <v>21518.444329946928</v>
       </c>
       <c r="K32" s="6">
-        <f>(K6-K8)/K12</f>
-        <v>17.24807618488882</v>
+        <f t="shared" si="1"/>
+        <v>23289.599924286253</v>
       </c>
       <c r="L32" s="6">
-        <f>(L6-L8)/L12</f>
-        <v>17.601382617249794</v>
+        <f t="shared" si="1"/>
+        <v>25052.811308240794</v>
       </c>
       <c r="M32" s="6">
-        <f>(M6-M8)/M12</f>
-        <v>17.927713863249643</v>
+        <f t="shared" si="1"/>
+        <v>26803.740790090687</v>
       </c>
       <c r="N32" s="6">
-        <f>(N6-N8)/N12</f>
-        <v>18.071145175365899</v>
+        <f t="shared" si="1"/>
+        <v>28287.546640238834</v>
       </c>
       <c r="O32" s="6">
-        <f>(O6-O8)/O12</f>
-        <v>18.36090121841093</v>
+        <f t="shared" si="1"/>
+        <v>29998.968362413761</v>
       </c>
       <c r="P32" s="6">
-        <f>(P6-P8)/P12</f>
-        <v>18.646798441494354</v>
+        <f t="shared" si="1"/>
+        <v>31824.408363214905</v>
       </c>
       <c r="Q32" s="6">
-        <f>(Q6-Q8)/Q12</f>
-        <v>18.928631593623837</v>
+        <f t="shared" si="1"/>
+        <v>33771.042894467108</v>
       </c>
       <c r="R32" s="6">
-        <f>(R6-R8)/R12</f>
-        <v>19.206112337133042</v>
+        <f t="shared" si="1"/>
+        <v>35845.047104820696</v>
       </c>
       <c r="S32" s="6">
-        <f>(S6-S8)/S12</f>
-        <v>19.479018861918302</v>
+        <f t="shared" si="1"/>
+        <v>38052.921904012364</v>
       </c>
       <c r="T32" s="6">
-        <f>(T6-T8)/T12</f>
-        <v>19.747193969683391</v>
+        <f t="shared" si="1"/>
+        <v>40401.533691005214</v>
       </c>
       <c r="U32" s="6">
-        <f>(U6-U8)/U12</f>
-        <v>20.010537791558178</v>
+        <f t="shared" si="1"/>
+        <v>42898.135447470006</v>
       </c>
       <c r="V32" s="6">
-        <f>(V6-V8)/V12</f>
-        <v>20.269000696548169</v>
+        <f t="shared" si="1"/>
+        <v>45550.388861367726</v>
       </c>
       <c r="W32" s="6">
-        <f>(W6-W8)/W12</f>
-        <v>20.522576564263439</v>
+        <f t="shared" si="1"/>
+        <v>48366.387755991331</v>
       </c>
       <c r="X32" s="6">
-        <f>(X6-X8)/X12</f>
-        <v>20.771296505457485</v>
+        <f t="shared" si="1"/>
+        <v>51354.682905464237</v>
       </c>
       <c r="Y32" s="6">
-        <f>(Y6-Y8)/Y12</f>
-        <v>21.015223081480574</v>
+        <f t="shared" si="1"/>
+        <v>54524.308320504642</v>
       </c>
       <c r="Z32" s="6">
-        <f>(Z6-Z8)/Z12</f>
-        <v>21.158046885294333</v>
+        <f t="shared" si="1"/>
+        <v>57622.276280895683</v>
       </c>
       <c r="AA32" s="6">
-        <f>(AA6-AA8)/AA12</f>
-        <v>21.397259297982067</v>
+        <f t="shared" si="1"/>
+        <v>61183.738084077064</v>
       </c>
       <c r="AB32" s="6">
-        <f>(AB6-AB8)/AB12</f>
-        <v>21.631805084163414</v>
+        <f t="shared" si="1"/>
+        <v>64956.818422587967</v>
       </c>
       <c r="AC32" s="6">
-        <f>(AC6-AC8)/AC12</f>
-        <v>21.861830719411188</v>
+        <f t="shared" si="1"/>
+        <v>68952.779746770728</v>
       </c>
       <c r="AD32" s="6">
-        <f>(AD6-AD8)/AD12</f>
-        <v>22.087493385435987</v>
+        <f t="shared" si="1"/>
+        <v>73183.524538208323</v>
       </c>
       <c r="AE32" s="6">
-        <f>(AE6-AE8)/AE12</f>
-        <v>22.308958046871801</v>
+        <f t="shared" si="1"/>
+        <v>77661.632488843446</v>
       </c>
       <c r="AF32" s="6">
-        <f>(AF6-AF8)/AF12</f>
-        <v>22.526394939838909</v>
+        <f t="shared" si="1"/>
+        <v>82400.399900637261</v>
       </c>
       <c r="AG32" s="6">
-        <f>(AG6-AG8)/AG12</f>
-        <v>22.7399774331518</v>
+        <f t="shared" si="1"/>
+        <v>87413.881440999219</v>
       </c>
       <c r="AH32" s="6">
-        <f>(AH6-AH8)/AH12</f>
-        <v>22.949880223520971</v>
+        <f t="shared" si="1"/>
+        <v>92716.934397586549</v>
       </c>
       <c r="AI32" s="6">
-        <f>(AI6-AI8)/AI12</f>
-        <v>23.156277827535803</v>
+        <f t="shared" si="1"/>
+        <v>98325.265584960929</v>
       </c>
       <c r="AJ32" s="6">
-        <f>(AJ6-AJ8)/AJ12</f>
-        <v>23.359343335303599</v>
+        <f t="shared" si="1"/>
+        <v>104255.48106503914</v>
       </c>
       <c r="AK32" s="6">
-        <f>(AK6-AK8)/AK12</f>
-        <v>23.559247393110795</v>
-      </c>
-    </row>
-    <row r="33" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>110525.13885331117</v>
+      </c>
+      <c r="AL32" s="6"/>
+    </row>
+    <row r="33" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -3435,157 +3467,159 @@
       <c r="AI33" s="6"/>
       <c r="AJ33" s="6"/>
       <c r="AK33" s="6"/>
-    </row>
-    <row r="34" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AL33" s="6"/>
+    </row>
+    <row r="34" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="6">
-        <f>B10/B12</f>
-        <v>13.653045796982603</v>
-      </c>
-      <c r="C34" s="6">
-        <f>C10/C12</f>
-        <v>12.226350099238815</v>
-      </c>
-      <c r="D34" s="6">
-        <f>D10/D12</f>
-        <v>11.075892602089247</v>
-      </c>
-      <c r="E34" s="6">
-        <f>E10/E12</f>
-        <v>10.12950548232147</v>
-      </c>
-      <c r="F34" s="6">
-        <f>F10/F12</f>
-        <v>9.3382342130200193</v>
-      </c>
-      <c r="G34" s="6">
-        <f>G10/G12</f>
-        <v>10.351393128021217</v>
-      </c>
-      <c r="H34" s="6">
-        <f>H10/H12</f>
-        <v>9.6620917139512308</v>
-      </c>
-      <c r="I34" s="6">
-        <f>I10/I12</f>
-        <v>9.0657960931821453</v>
-      </c>
-      <c r="J34" s="6">
-        <f>J10/J12</f>
-        <v>8.545863394730544</v>
-      </c>
-      <c r="K34" s="6">
-        <f>K10/K12</f>
-        <v>8.0894987353417136</v>
-      </c>
-      <c r="L34" s="6">
-        <f>L10/L12</f>
-        <v>7.6867161385696763</v>
-      </c>
-      <c r="M34" s="6">
-        <f>M10/M12</f>
-        <v>15.335769596970753</v>
-      </c>
-      <c r="N34" s="6">
-        <f>N10/N12</f>
-        <v>8.8577643562576007</v>
-      </c>
-      <c r="O34" s="6">
-        <f>O10/O12</f>
-        <v>8.4969396785771742</v>
-      </c>
-      <c r="P34" s="6">
-        <f>P10/P12</f>
-        <v>8.14507782216997</v>
-      </c>
-      <c r="Q34" s="6">
-        <f>Q10/Q12</f>
-        <v>7.8026102678591123</v>
-      </c>
-      <c r="R34" s="6">
-        <f>R10/R12</f>
-        <v>8.5695172415170333</v>
-      </c>
-      <c r="S34" s="6">
-        <f>S10/S12</f>
-        <v>8.1984222512261677</v>
-      </c>
-      <c r="T34" s="6">
-        <f>T10/T12</f>
-        <v>7.8397384140255735</v>
-      </c>
-      <c r="U34" s="6">
-        <f>U10/U12</f>
-        <v>7.4937061122780735</v>
-      </c>
-      <c r="V34" s="6">
-        <f>V10/V12</f>
-        <v>7.1604481918356431</v>
-      </c>
-      <c r="W34" s="6">
-        <f>W10/W12</f>
-        <v>6.8399857061207019</v>
-      </c>
-      <c r="X34" s="6">
-        <f>X10/X12</f>
-        <v>6.5322526121470581</v>
-      </c>
-      <c r="Y34" s="6">
-        <f>Y10/Y12</f>
-        <v>15.925625831633358</v>
-      </c>
-      <c r="Z34" s="6">
-        <f>Z10/Z12</f>
-        <v>6.1818140705486373</v>
-      </c>
-      <c r="AA34" s="6">
-        <f>AA10/AA12</f>
-        <v>5.9003792021508978</v>
-      </c>
-      <c r="AB34" s="6">
-        <f>AB10/AB12</f>
-        <v>5.63126197858921</v>
-      </c>
-      <c r="AC34" s="6">
-        <f>AC10/AC12</f>
-        <v>5.3741264437072305</v>
-      </c>
-      <c r="AD34" s="6">
-        <f>AD10/AD12</f>
-        <v>5.1286116142794418</v>
-      </c>
-      <c r="AE34" s="6">
-        <f>AE10/AE12</f>
-        <v>4.8943383234311248</v>
-      </c>
-      <c r="AF34" s="6">
-        <f>AF10/AF12</f>
-        <v>4.6709151000733833</v>
-      </c>
-      <c r="AG34" s="6">
-        <f>AG10/AG12</f>
-        <v>4.4579431759651369</v>
-      </c>
-      <c r="AH34" s="6">
-        <f>AH10/AH12</f>
-        <v>4.2550207108875124</v>
-      </c>
-      <c r="AI34" s="6">
-        <f>AI10/AI12</f>
-        <v>4.061746323047533</v>
-      </c>
-      <c r="AJ34" s="6">
-        <f>AJ10/AJ12</f>
-        <v>3.8777220069413705</v>
-      </c>
-      <c r="AK34" s="6">
-        <f>AK10/AK12</f>
-        <v>9.5506797056406487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B34" s="7">
+        <f>B32/B12</f>
+        <v>13.989181645836057</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" ref="C34:AK34" si="2">C32/C12</f>
+        <v>14.841496961572126</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="2"/>
+        <v>15.549784949153652</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="2"/>
+        <v>16.151804880276416</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" si="2"/>
+        <v>16.673179435248599</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="2"/>
+        <v>15.448216578622993</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="2"/>
+        <v>15.971976550004259</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="2"/>
+        <v>16.440239087149006</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="2"/>
+        <v>16.863034909542908</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="2"/>
+        <v>17.24807618488882</v>
+      </c>
+      <c r="L34" s="7">
+        <f t="shared" si="2"/>
+        <v>17.601382617249794</v>
+      </c>
+      <c r="M34" s="7">
+        <f t="shared" si="2"/>
+        <v>17.927713863249643</v>
+      </c>
+      <c r="N34" s="7">
+        <f t="shared" si="2"/>
+        <v>18.071145175365899</v>
+      </c>
+      <c r="O34" s="7">
+        <f t="shared" si="2"/>
+        <v>18.36090121841093</v>
+      </c>
+      <c r="P34" s="7">
+        <f t="shared" si="2"/>
+        <v>18.646798441494354</v>
+      </c>
+      <c r="Q34" s="7">
+        <f t="shared" si="2"/>
+        <v>18.928631593623837</v>
+      </c>
+      <c r="R34" s="7">
+        <f t="shared" si="2"/>
+        <v>19.206112337133042</v>
+      </c>
+      <c r="S34" s="7">
+        <f t="shared" si="2"/>
+        <v>19.479018861918302</v>
+      </c>
+      <c r="T34" s="7">
+        <f t="shared" si="2"/>
+        <v>19.747193969683391</v>
+      </c>
+      <c r="U34" s="7">
+        <f t="shared" si="2"/>
+        <v>20.010537791558178</v>
+      </c>
+      <c r="V34" s="7">
+        <f t="shared" si="2"/>
+        <v>20.269000696548169</v>
+      </c>
+      <c r="W34" s="7">
+        <f t="shared" si="2"/>
+        <v>20.522576564263439</v>
+      </c>
+      <c r="X34" s="7">
+        <f t="shared" si="2"/>
+        <v>20.771296505457485</v>
+      </c>
+      <c r="Y34" s="7">
+        <f t="shared" si="2"/>
+        <v>21.015223081480574</v>
+      </c>
+      <c r="Z34" s="7">
+        <f t="shared" si="2"/>
+        <v>21.158046885294333</v>
+      </c>
+      <c r="AA34" s="7">
+        <f t="shared" si="2"/>
+        <v>21.397259297982067</v>
+      </c>
+      <c r="AB34" s="7">
+        <f t="shared" si="2"/>
+        <v>21.631805084163414</v>
+      </c>
+      <c r="AC34" s="7">
+        <f t="shared" si="2"/>
+        <v>21.861830719411188</v>
+      </c>
+      <c r="AD34" s="7">
+        <f t="shared" si="2"/>
+        <v>22.087493385435987</v>
+      </c>
+      <c r="AE34" s="7">
+        <f t="shared" si="2"/>
+        <v>22.308958046871801</v>
+      </c>
+      <c r="AF34" s="7">
+        <f t="shared" si="2"/>
+        <v>22.526394939838909</v>
+      </c>
+      <c r="AG34" s="7">
+        <f t="shared" si="2"/>
+        <v>22.7399774331518</v>
+      </c>
+      <c r="AH34" s="7">
+        <f t="shared" si="2"/>
+        <v>22.949880223520971</v>
+      </c>
+      <c r="AI34" s="7">
+        <f t="shared" si="2"/>
+        <v>23.156277827535803</v>
+      </c>
+      <c r="AJ34" s="7">
+        <f t="shared" si="2"/>
+        <v>23.359343335303599</v>
+      </c>
+      <c r="AK34" s="7">
+        <f t="shared" si="2"/>
+        <v>23.559247393110795</v>
+      </c>
+      <c r="AL34" s="7"/>
+    </row>
+    <row r="35" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -3622,157 +3656,159 @@
       <c r="AI35" s="8"/>
       <c r="AJ35" s="8"/>
       <c r="AK35" s="8"/>
-    </row>
-    <row r="36" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AL35" s="8"/>
+    </row>
+    <row r="36" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B36" s="18">
-        <f>B32*B28</f>
-        <v>12.492200225697035</v>
+        <f>B10/B12</f>
+        <v>13.653045796982603</v>
       </c>
       <c r="C36" s="18">
-        <f t="shared" ref="C36:AK36" si="1">C32*C28</f>
-        <v>11.863102504507657</v>
+        <f t="shared" ref="C36:AK36" si="3">C10/C12</f>
+        <v>12.226350099238815</v>
       </c>
       <c r="D36" s="18">
-        <f t="shared" si="1"/>
-        <v>11.15183236191133</v>
+        <f t="shared" si="3"/>
+        <v>11.075892602089247</v>
       </c>
       <c r="E36" s="18">
-        <f t="shared" si="1"/>
-        <v>10.417691575672421</v>
+        <f t="shared" si="3"/>
+        <v>10.12950548232147</v>
       </c>
       <c r="F36" s="18">
-        <f t="shared" si="1"/>
-        <v>9.6944856557801842</v>
+        <f t="shared" si="3"/>
+        <v>9.3382342130200193</v>
       </c>
       <c r="G36" s="18">
-        <f t="shared" si="1"/>
-        <v>8.1164838968582398</v>
+        <f t="shared" si="3"/>
+        <v>10.351393128021217</v>
       </c>
       <c r="H36" s="18">
-        <f t="shared" si="1"/>
-        <v>7.6007911704053992</v>
+        <f t="shared" si="3"/>
+        <v>9.6620917139512308</v>
       </c>
       <c r="I36" s="18">
-        <f t="shared" si="1"/>
-        <v>7.1030707730966558</v>
+        <f t="shared" si="3"/>
+        <v>9.0657960931821453</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="1"/>
-        <v>6.6303880893625999</v>
+        <f t="shared" si="3"/>
+        <v>8.545863394730544</v>
       </c>
       <c r="K36" s="18">
-        <f t="shared" si="1"/>
-        <v>6.1863771151238023</v>
+        <f t="shared" si="3"/>
+        <v>8.0894987353417136</v>
       </c>
       <c r="L36" s="18">
-        <f t="shared" si="1"/>
-        <v>5.7724788778894114</v>
+        <f t="shared" si="3"/>
+        <v>7.6867161385696763</v>
       </c>
       <c r="M36" s="18">
-        <f t="shared" si="1"/>
-        <v>5.3887451128574417</v>
+        <f t="shared" si="3"/>
+        <v>15.335769596970753</v>
       </c>
       <c r="N36" s="18">
-        <f t="shared" si="1"/>
-        <v>4.9902567109364258</v>
+        <f t="shared" si="3"/>
+        <v>8.8577643562576007</v>
       </c>
       <c r="O36" s="18">
-        <f t="shared" si="1"/>
-        <v>4.6690982254646745</v>
+        <f t="shared" si="3"/>
+        <v>8.4969396785771742</v>
       </c>
       <c r="P36" s="18">
-        <f t="shared" si="1"/>
-        <v>4.3769583888077852</v>
+        <f t="shared" si="3"/>
+        <v>8.14507782216997</v>
       </c>
       <c r="Q36" s="18">
-        <f t="shared" si="1"/>
-        <v>4.1109652571648061</v>
+        <f t="shared" si="3"/>
+        <v>7.8026102678591123</v>
       </c>
       <c r="R36" s="18">
-        <f t="shared" si="1"/>
-        <v>3.8685464886617411</v>
+        <f t="shared" si="3"/>
+        <v>8.5695172415170333</v>
       </c>
       <c r="S36" s="18">
-        <f t="shared" si="1"/>
-        <v>3.6474262767057093</v>
+        <f t="shared" si="3"/>
+        <v>8.1984222512261677</v>
       </c>
       <c r="T36" s="18">
-        <f t="shared" si="1"/>
-        <v>3.4455872105135752</v>
+        <f t="shared" si="3"/>
+        <v>7.8397384140255735</v>
       </c>
       <c r="U36" s="18">
-        <f t="shared" si="1"/>
-        <v>3.2612368936943432</v>
+        <f t="shared" si="3"/>
+        <v>7.4937061122780735</v>
       </c>
       <c r="V36" s="18">
-        <f t="shared" si="1"/>
-        <v>3.0927796316624216</v>
+        <f t="shared" si="3"/>
+        <v>7.1604481918356431</v>
       </c>
       <c r="W36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.9387923291788849</v>
+        <f t="shared" si="3"/>
+        <v>6.8399857061207019</v>
       </c>
       <c r="X36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.7980038877650149</v>
+        <f t="shared" si="3"/>
+        <v>6.5322526121470581</v>
       </c>
       <c r="Y36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.6692775234974739</v>
+        <f t="shared" si="3"/>
+        <v>15.925625831633358</v>
       </c>
       <c r="Z36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.5400229353129578</v>
+        <f t="shared" si="3"/>
+        <v>6.1818140705486373</v>
       </c>
       <c r="AA36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.4336037828576123</v>
+        <f t="shared" si="3"/>
+        <v>5.9003792021508978</v>
       </c>
       <c r="AB36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.3363691533824724</v>
+        <f t="shared" si="3"/>
+        <v>5.63126197858921</v>
       </c>
       <c r="AC36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.247602630079665</v>
+        <f t="shared" si="3"/>
+        <v>5.3741264437072305</v>
       </c>
       <c r="AD36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.1666614686074475</v>
+        <f t="shared" si="3"/>
+        <v>5.1286116142794418</v>
       </c>
       <c r="AE36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.0929693028803986</v>
+        <f t="shared" si="3"/>
+        <v>4.8943383234311248</v>
       </c>
       <c r="AF36" s="18">
-        <f t="shared" si="1"/>
-        <v>2.0260097525639496</v>
+        <f t="shared" si="3"/>
+        <v>4.6709151000733833</v>
       </c>
       <c r="AG36" s="18">
-        <f t="shared" si="1"/>
-        <v>1.9653208149731882</v>
+        <f t="shared" si="3"/>
+        <v>4.4579431759651369</v>
       </c>
       <c r="AH36" s="18">
-        <f t="shared" si="1"/>
-        <v>1.9104899434842584</v>
+        <f t="shared" si="3"/>
+        <v>4.2550207108875124</v>
       </c>
       <c r="AI36" s="18">
-        <f t="shared" si="1"/>
-        <v>1.8611497304907283</v>
+        <f t="shared" si="3"/>
+        <v>4.061746323047533</v>
       </c>
       <c r="AJ36" s="18">
-        <f t="shared" si="1"/>
-        <v>1.8169741260867658</v>
+        <f t="shared" si="3"/>
+        <v>3.8777220069413705</v>
       </c>
       <c r="AK36" s="18">
-        <f t="shared" si="1"/>
-        <v>1.7776751345998321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>9.5506797056406487</v>
+      </c>
+      <c r="AL36" s="18"/>
+    </row>
+    <row r="37" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -3809,157 +3845,159 @@
       <c r="AI37" s="8"/>
       <c r="AJ37" s="8"/>
       <c r="AK37" s="8"/>
-    </row>
-    <row r="38" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AL37" s="8"/>
+    </row>
+    <row r="38" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B38" s="7">
-        <f>B34*B30</f>
-        <v>12.197209244507535</v>
+        <f>B34*B28</f>
+        <v>12.492200225697035</v>
       </c>
       <c r="C38" s="7">
-        <f t="shared" ref="C38:AK38" si="2">C34*C30</f>
-        <v>9.7769119325451719</v>
+        <f t="shared" ref="C38:AK38" si="4">C34*C28</f>
+        <v>11.863102504507657</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="2"/>
-        <v>7.9466645605012944</v>
+        <f t="shared" si="4"/>
+        <v>11.15183236191133</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" si="2"/>
-        <v>6.5361645940324662</v>
+        <f t="shared" si="4"/>
+        <v>10.417691575672421</v>
       </c>
       <c r="F38" s="7">
-        <f t="shared" si="2"/>
-        <v>5.4319455862280588</v>
+        <f t="shared" si="4"/>
+        <v>9.6944856557801842</v>
       </c>
       <c r="G38" s="7">
-        <f t="shared" si="2"/>
-        <v>5.4409243138250529</v>
+        <f t="shared" si="4"/>
+        <v>8.1164838968582398</v>
       </c>
       <c r="H38" s="7">
-        <f t="shared" si="2"/>
-        <v>4.5999762817362502</v>
+        <f t="shared" si="4"/>
+        <v>7.6007911704053992</v>
       </c>
       <c r="I38" s="7">
-        <f t="shared" si="2"/>
-        <v>3.9185758684604144</v>
+        <f t="shared" si="4"/>
+        <v>7.1030707730966558</v>
       </c>
       <c r="J38" s="7">
-        <f t="shared" si="2"/>
-        <v>3.3615800423234501</v>
+        <f t="shared" si="4"/>
+        <v>6.6303880893625999</v>
       </c>
       <c r="K38" s="7">
-        <f t="shared" si="2"/>
-        <v>2.9026965745748949</v>
+        <f t="shared" si="4"/>
+        <v>6.1863771151238023</v>
       </c>
       <c r="L38" s="7">
-        <f t="shared" si="2"/>
-        <v>2.5219746233788469</v>
+        <f t="shared" si="4"/>
+        <v>5.7724788778894114</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" si="2"/>
-        <v>4.6116103506628958</v>
+        <f t="shared" si="4"/>
+        <v>5.3887451128574417</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" si="2"/>
-        <v>2.4470657312830131</v>
+        <f t="shared" si="4"/>
+        <v>4.9902567109364258</v>
       </c>
       <c r="O38" s="7">
-        <f t="shared" si="2"/>
-        <v>2.1616523611009075</v>
+        <f t="shared" si="4"/>
+        <v>4.6690982254646745</v>
       </c>
       <c r="P38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.9127036194633755</v>
+        <f t="shared" si="4"/>
+        <v>4.3769583888077852</v>
       </c>
       <c r="Q38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6953087472477208</v>
+        <f t="shared" si="4"/>
+        <v>4.1109652571648061</v>
       </c>
       <c r="R38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7268277236451419</v>
+        <f t="shared" si="4"/>
+        <v>3.8685464886617411</v>
       </c>
       <c r="S38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5357977499402213</v>
+        <f t="shared" si="4"/>
+        <v>3.6474262767057093</v>
       </c>
       <c r="T38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.3684966125288478</v>
+        <f t="shared" si="4"/>
+        <v>3.4455872105135752</v>
       </c>
       <c r="U38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.2218124416952141</v>
+        <f t="shared" si="4"/>
+        <v>3.2612368936943432</v>
       </c>
       <c r="V38" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0930528121135161</v>
+        <f t="shared" si="4"/>
+        <v>3.0927796316624216</v>
       </c>
       <c r="W38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.97988815366476978</v>
+        <f t="shared" si="4"/>
+        <v>2.9387923291788849</v>
       </c>
       <c r="X38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.88030259022543456</v>
+        <f t="shared" si="4"/>
+        <v>2.7980038877650149</v>
       </c>
       <c r="Y38" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0236739119636846</v>
+        <f t="shared" si="4"/>
+        <v>2.6692775234974739</v>
       </c>
       <c r="Z38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.74244160654423996</v>
+        <f t="shared" si="4"/>
+        <v>2.5400229353129578</v>
       </c>
       <c r="AA38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.67136074769665854</v>
+        <f t="shared" si="4"/>
+        <v>2.4336037828576123</v>
       </c>
       <c r="AB38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.60846938960115515</v>
+        <f t="shared" si="4"/>
+        <v>2.3363691533824724</v>
       </c>
       <c r="AC38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.5527454610889897</v>
+        <f t="shared" si="4"/>
+        <v>2.247602630079665</v>
       </c>
       <c r="AD38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.50330209624544986</v>
+        <f t="shared" si="4"/>
+        <v>2.1666614686074475</v>
       </c>
       <c r="AE38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.45936918504945717</v>
+        <f t="shared" si="4"/>
+        <v>2.0929693028803986</v>
       </c>
       <c r="AF38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.42027747192170234</v>
+        <f t="shared" si="4"/>
+        <v>2.0260097525639496</v>
       </c>
       <c r="AG38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.38544485500332204</v>
+        <f t="shared" si="4"/>
+        <v>1.9653208149731882</v>
       </c>
       <c r="AH38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.35436458412235805</v>
+        <f t="shared" si="4"/>
+        <v>1.9104899434842584</v>
       </c>
       <c r="AI38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.3265950952875849</v>
+        <f t="shared" si="4"/>
+        <v>1.8611497304907283</v>
       </c>
       <c r="AJ38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.30175125464144215</v>
+        <f t="shared" si="4"/>
+        <v>1.8169741260867658</v>
       </c>
       <c r="AK38" s="7">
-        <f t="shared" si="2"/>
-        <v>0.72095733698431363</v>
-      </c>
-    </row>
-    <row r="39" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.7776751345998321</v>
+      </c>
+      <c r="AL38" s="7"/>
+    </row>
+    <row r="39" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -3996,182 +4034,342 @@
       <c r="AI39" s="6"/>
       <c r="AJ39" s="6"/>
       <c r="AK39" s="6"/>
-    </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL39" s="6"/>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1">
-        <f>B36-B38</f>
+        <f>B36*B30</f>
+        <v>12.197209244507535</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" ref="C40:AK40" si="5">C36*C30</f>
+        <v>9.7769119325451719</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="5"/>
+        <v>7.9466645605012944</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="5"/>
+        <v>6.5361645940324662</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="5"/>
+        <v>5.4319455862280588</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="5"/>
+        <v>5.4409243138250529</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="5"/>
+        <v>4.5999762817362502</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="5"/>
+        <v>3.9185758684604144</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="5"/>
+        <v>3.3615800423234501</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.9026965745748949</v>
+      </c>
+      <c r="L40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.5219746233788469</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="5"/>
+        <v>4.6116103506628958</v>
+      </c>
+      <c r="N40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.4470657312830131</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.1616523611009075</v>
+      </c>
+      <c r="P40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.9127036194633755</v>
+      </c>
+      <c r="Q40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.6953087472477208</v>
+      </c>
+      <c r="R40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7268277236451419</v>
+      </c>
+      <c r="S40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.5357977499402213</v>
+      </c>
+      <c r="T40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.3684966125288478</v>
+      </c>
+      <c r="U40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2218124416952141</v>
+      </c>
+      <c r="V40" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0930528121135161</v>
+      </c>
+      <c r="W40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.97988815366476978</v>
+      </c>
+      <c r="X40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.88030259022543456</v>
+      </c>
+      <c r="Y40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.0236739119636846</v>
+      </c>
+      <c r="Z40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.74244160654423996</v>
+      </c>
+      <c r="AA40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.67136074769665854</v>
+      </c>
+      <c r="AB40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.60846938960115515</v>
+      </c>
+      <c r="AC40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5527454610889897</v>
+      </c>
+      <c r="AD40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.50330209624544986</v>
+      </c>
+      <c r="AE40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.45936918504945717</v>
+      </c>
+      <c r="AF40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.42027747192170234</v>
+      </c>
+      <c r="AG40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.38544485500332204</v>
+      </c>
+      <c r="AH40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.35436458412235805</v>
+      </c>
+      <c r="AI40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.3265950952875849</v>
+      </c>
+      <c r="AJ40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.30175125464144215</v>
+      </c>
+      <c r="AK40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.72095733698431363</v>
+      </c>
+      <c r="AL40" s="1"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1">
+        <f>B38-B40</f>
         <v>0.29499098118949973</v>
       </c>
-      <c r="C40" s="1">
-        <f t="shared" ref="C40:AK40" si="3">C36-C38</f>
+      <c r="C42" s="1">
+        <f t="shared" ref="C42:AK42" si="6">C38-C40</f>
         <v>2.0861905719624847</v>
       </c>
-      <c r="D40" s="1">
-        <f t="shared" si="3"/>
+      <c r="D42" s="1">
+        <f t="shared" si="6"/>
         <v>3.2051678014100355</v>
       </c>
-      <c r="E40" s="1">
-        <f t="shared" si="3"/>
+      <c r="E42" s="1">
+        <f t="shared" si="6"/>
         <v>3.8815269816399551</v>
       </c>
-      <c r="F40" s="1">
-        <f t="shared" si="3"/>
+      <c r="F42" s="1">
+        <f t="shared" si="6"/>
         <v>4.2625400695521254</v>
       </c>
-      <c r="G40" s="1">
-        <f t="shared" si="3"/>
+      <c r="G42" s="1">
+        <f t="shared" si="6"/>
         <v>2.6755595830331869</v>
       </c>
-      <c r="H40" s="1">
-        <f t="shared" si="3"/>
+      <c r="H42" s="1">
+        <f t="shared" si="6"/>
         <v>3.000814888669149</v>
       </c>
-      <c r="I40" s="1">
-        <f t="shared" si="3"/>
+      <c r="I42" s="1">
+        <f t="shared" si="6"/>
         <v>3.1844949046362414</v>
       </c>
-      <c r="J40" s="1">
-        <f t="shared" si="3"/>
+      <c r="J42" s="1">
+        <f t="shared" si="6"/>
         <v>3.2688080470391498</v>
       </c>
-      <c r="K40" s="1">
-        <f t="shared" si="3"/>
+      <c r="K42" s="1">
+        <f t="shared" si="6"/>
         <v>3.2836805405489073</v>
       </c>
-      <c r="L40" s="1">
-        <f t="shared" si="3"/>
+      <c r="L42" s="1">
+        <f t="shared" si="6"/>
         <v>3.2505042545105645</v>
       </c>
-      <c r="M40" s="1">
-        <f t="shared" si="3"/>
+      <c r="M42" s="1">
+        <f t="shared" si="6"/>
         <v>0.77713476219454591</v>
       </c>
-      <c r="N40" s="1">
-        <f t="shared" si="3"/>
+      <c r="N42" s="1">
+        <f t="shared" si="6"/>
         <v>2.5431909796534127</v>
       </c>
-      <c r="O40" s="1">
-        <f t="shared" si="3"/>
+      <c r="O42" s="1">
+        <f t="shared" si="6"/>
         <v>2.5074458643637669</v>
       </c>
-      <c r="P40" s="1">
-        <f t="shared" si="3"/>
+      <c r="P42" s="1">
+        <f t="shared" si="6"/>
         <v>2.4642547693444099</v>
       </c>
-      <c r="Q40" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q42" s="1">
+        <f t="shared" si="6"/>
         <v>2.4156565099170852</v>
       </c>
-      <c r="R40" s="1">
-        <f t="shared" si="3"/>
+      <c r="R42" s="1">
+        <f t="shared" si="6"/>
         <v>2.1417187650165994</v>
       </c>
-      <c r="S40" s="1">
-        <f t="shared" si="3"/>
+      <c r="S42" s="1">
+        <f t="shared" si="6"/>
         <v>2.1116285267654877</v>
       </c>
-      <c r="T40" s="1">
-        <f t="shared" si="3"/>
+      <c r="T42" s="1">
+        <f t="shared" si="6"/>
         <v>2.0770905979847276</v>
       </c>
-      <c r="U40" s="1">
-        <f t="shared" si="3"/>
+      <c r="U42" s="1">
+        <f t="shared" si="6"/>
         <v>2.0394244519991291</v>
       </c>
-      <c r="V40" s="1">
-        <f t="shared" si="3"/>
+      <c r="V42" s="1">
+        <f t="shared" si="6"/>
         <v>1.9997268195489055</v>
       </c>
-      <c r="W40" s="1">
-        <f t="shared" si="3"/>
+      <c r="W42" s="1">
+        <f t="shared" si="6"/>
         <v>1.9589041755141152</v>
       </c>
-      <c r="X40" s="1">
-        <f t="shared" si="3"/>
+      <c r="X42" s="1">
+        <f t="shared" si="6"/>
         <v>1.9177012975395802</v>
       </c>
-      <c r="Y40" s="1">
-        <f t="shared" si="3"/>
+      <c r="Y42" s="1">
+        <f t="shared" si="6"/>
         <v>0.64560361153378931</v>
       </c>
-      <c r="Z40" s="1">
-        <f t="shared" si="3"/>
+      <c r="Z42" s="1">
+        <f t="shared" si="6"/>
         <v>1.7975813287687177</v>
       </c>
-      <c r="AA40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AA42" s="1">
+        <f t="shared" si="6"/>
         <v>1.7622430351609537</v>
       </c>
-      <c r="AB40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AB42" s="1">
+        <f t="shared" si="6"/>
         <v>1.7278997637813172</v>
       </c>
-      <c r="AC40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AC42" s="1">
+        <f t="shared" si="6"/>
         <v>1.6948571689906753</v>
       </c>
-      <c r="AD40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AD42" s="1">
+        <f t="shared" si="6"/>
         <v>1.6633593723619975</v>
       </c>
-      <c r="AE40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AE42" s="1">
+        <f t="shared" si="6"/>
         <v>1.6336001178309414</v>
       </c>
-      <c r="AF40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AF42" s="1">
+        <f t="shared" si="6"/>
         <v>1.6057322806422472</v>
       </c>
-      <c r="AG40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AG42" s="1">
+        <f t="shared" si="6"/>
         <v>1.5798759599698662</v>
       </c>
-      <c r="AH40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AH42" s="1">
+        <f t="shared" si="6"/>
         <v>1.5561253593619004</v>
       </c>
-      <c r="AI40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AI42" s="1">
+        <f t="shared" si="6"/>
         <v>1.5345546352031434</v>
       </c>
-      <c r="AJ40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AJ42" s="1">
+        <f t="shared" si="6"/>
         <v>1.5152228714453235</v>
       </c>
-      <c r="AK40" s="1">
-        <f t="shared" si="3"/>
+      <c r="AK42" s="1">
+        <f t="shared" si="6"/>
         <v>1.0567177976155184</v>
       </c>
-    </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="AL42" s="1"/>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="1">
+        <f>SUM(B42:AK42)</f>
+        <v>77.121529446699441</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="28">
+        <f>B44/3</f>
+        <v>25.707176482233148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="1">
-        <f>SUM(B40:AK40)</f>
-        <v>77.121529446699441</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="1">
-        <f>B42/3</f>
-        <v>25.707176482233148</v>
-      </c>
-    </row>
-    <row r="44" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="22">
-        <f>B42+B43</f>
+      <c r="B46" s="22">
+        <f>B44+B45</f>
         <v>102.82870592893259</v>
       </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>